<commit_message>
Better readable legends in plots
</commit_message>
<xml_diff>
--- a/final assignment/data/robustness_results/overall_scores.xlsx
+++ b/final assignment/data/robustness_results/overall_scores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Final epsilons and remove dike_model_optimization
</commit_message>
<xml_diff>
--- a/final assignment/data/robustness_results/overall_scores.xlsx
+++ b/final assignment/data/robustness_results/overall_scores.xlsx
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.535</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -536,7 +536,7 @@
         <v>0.849</v>
       </c>
       <c r="E2" t="n">
-        <v>0.132</v>
+        <v>0.293</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0.41</v>
+        <v>0.525</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -554,16 +554,16 @@
         <v>0.924</v>
       </c>
       <c r="K2" t="n">
-        <v>0.539</v>
+        <v>0.707</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
       </c>
       <c r="N2" t="n">
-        <v>0.653</v>
+        <v>0.716</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>1</v>
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.828</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -594,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08500000000000001</v>
+        <v>0.317</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.276</v>
+        <v>0.437</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -612,16 +612,16 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0.71</v>
+        <v>0.853</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0.718</v>
+        <v>0.763</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.535</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.099</v>
+        <v>0.165</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -661,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0.288</v>
+        <v>0.323</v>
       </c>
       <c r="I4" t="n">
         <v>1</v>
@@ -670,7 +670,7 @@
         <v>0.827</v>
       </c>
       <c r="K4" t="n">
-        <v>0.569</v>
+        <v>0.67</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -679,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>0.718</v>
+        <v>0.739</v>
       </c>
       <c r="O4" t="n">
         <v>1</v>
@@ -701,7 +701,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.93</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>0.658</v>
+        <v>0.796</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.767</v>
+        <v>0.854</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -728,7 +728,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0.903</v>
+        <v>0.978</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="n">
-        <v>0.152</v>
+        <v>0.235</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.964</v>
+        <v>0.971</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9320000000000001</v>
+        <v>0.965</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.166</v>
+        <v>0.328</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>0.944</v>
+        <v>0.99</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -795,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="n">
-        <v>0.158</v>
+        <v>0.2</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.866</v>
+        <v>0.877</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -826,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.674</v>
+        <v>0.803</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -835,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.468</v>
+        <v>0.591</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -844,7 +844,7 @@
         <v>0.987</v>
       </c>
       <c r="K7" t="n">
-        <v>0.633</v>
+        <v>0.867</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="n">
-        <v>0.377</v>
+        <v>0.502</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.883</v>
+        <v>0.91</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -884,7 +884,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>0.711</v>
+        <v>0.841</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0.946</v>
+        <v>0.975</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.9419999999999999</v>
+        <v>0.993</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>0.635</v>
+        <v>0.845</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
@@ -933,7 +933,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.173</v>
+        <v>0.205</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -942,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>0.843</v>
+        <v>0.908</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0.764</v>
+        <v>0.861</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -960,7 +960,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.963</v>
+        <v>0.994</v>
       </c>
       <c r="L9" t="n">
         <v>0</v>
@@ -969,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="n">
-        <v>0.635</v>
+        <v>0.728</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.535</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.788</v>
+        <v>0.876</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0.927</v>
+        <v>0.953</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -1018,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.788</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="N10" t="n">
-        <v>0.579</v>
+        <v>0.694</v>
       </c>
       <c r="O10" t="n">
         <v>1</v>
@@ -1049,7 +1049,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.868</v>
+        <v>0.902</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1058,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.821</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -1067,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0.706</v>
+        <v>0.856</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1076,7 +1076,7 @@
         <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="N11" t="n">
-        <v>0.275</v>
+        <v>0.457</v>
       </c>
       <c r="O11" t="n">
         <v>0</v>

</xml_diff>